<commit_message>
data filtered out for update
</commit_message>
<xml_diff>
--- a/filterted_new_employee_list.xlsx
+++ b/filterted_new_employee_list.xlsx
@@ -5522,8 +5522,8 @@
   </sheetPr>
   <dimension ref="A1:AU192"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G9:G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D93" activeCellId="0" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>